<commit_message>
Adding pickling to replication
</commit_message>
<xml_diff>
--- a/replication/temp/figureA1_any_evidence.xlsx
+++ b/replication/temp/figureA1_any_evidence.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -34,7 +34,64 @@
     <t>total_dof</t>
   </si>
   <si>
-    <t>(nan)</t>
+    <t>(0.28)</t>
+  </si>
+  <si>
+    <t>(0.16)</t>
+  </si>
+  <si>
+    <t>(0.17)</t>
+  </si>
+  <si>
+    <t>(0.1)</t>
+  </si>
+  <si>
+    <t>(0.39)</t>
+  </si>
+  <si>
+    <t>(0.29)</t>
+  </si>
+  <si>
+    <t>(0.61)</t>
+  </si>
+  <si>
+    <t>(0.14)</t>
+  </si>
+  <si>
+    <t>(0.83)</t>
+  </si>
+  <si>
+    <t>(0.12)</t>
+  </si>
+  <si>
+    <t>(0.64)</t>
+  </si>
+  <si>
+    <t>(1.0)</t>
+  </si>
+  <si>
+    <t>(0.71)</t>
+  </si>
+  <si>
+    <t>(0.68)</t>
+  </si>
+  <si>
+    <t>(0.07)</t>
+  </si>
+  <si>
+    <t>(0.36)</t>
+  </si>
+  <si>
+    <t>(0.18)</t>
+  </si>
+  <si>
+    <t>(0.5)</t>
+  </si>
+  <si>
+    <t>(0.38)</t>
+  </si>
+  <si>
+    <t>(0.97)</t>
   </si>
 </sst>
 </file>
@@ -517,34 +574,34 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="I4" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="L4" t="s">
-        <v>6</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -590,37 +647,37 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
         <v>6</v>
       </c>
       <c r="G6" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="H6" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="I6" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K6" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="L6" t="s">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:12">

</xml_diff>

<commit_message>
Finishing replicate updates and testing
</commit_message>
<xml_diff>
--- a/replication/temp/figureA1_any_evidence.xlsx
+++ b/replication/temp/figureA1_any_evidence.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>year</t>
   </si>
@@ -34,64 +34,67 @@
     <t>total_dof</t>
   </si>
   <si>
-    <t>(0.28)</t>
-  </si>
-  <si>
-    <t>(0.16)</t>
-  </si>
-  <si>
-    <t>(0.17)</t>
+    <t>(0.42)</t>
+  </si>
+  <si>
+    <t>(0.01)</t>
+  </si>
+  <si>
+    <t>(0.41)</t>
+  </si>
+  <si>
+    <t>(0.26)</t>
+  </si>
+  <si>
+    <t>(0.49)</t>
+  </si>
+  <si>
+    <t>(0.15)</t>
+  </si>
+  <si>
+    <t>(1.0)</t>
+  </si>
+  <si>
+    <t>(0.3)</t>
+  </si>
+  <si>
+    <t>(0.44)</t>
+  </si>
+  <si>
+    <t>(0.02)</t>
   </si>
   <si>
     <t>(0.1)</t>
   </si>
   <si>
-    <t>(0.39)</t>
-  </si>
-  <si>
-    <t>(0.29)</t>
-  </si>
-  <si>
-    <t>(0.61)</t>
-  </si>
-  <si>
-    <t>(0.14)</t>
-  </si>
-  <si>
-    <t>(0.83)</t>
-  </si>
-  <si>
-    <t>(0.12)</t>
-  </si>
-  <si>
-    <t>(0.64)</t>
-  </si>
-  <si>
-    <t>(1.0)</t>
-  </si>
-  <si>
-    <t>(0.71)</t>
-  </si>
-  <si>
-    <t>(0.68)</t>
-  </si>
-  <si>
-    <t>(0.07)</t>
-  </si>
-  <si>
-    <t>(0.36)</t>
-  </si>
-  <si>
-    <t>(0.18)</t>
-  </si>
-  <si>
-    <t>(0.5)</t>
+    <t>(0.35)</t>
+  </si>
+  <si>
+    <t>(0.24)</t>
+  </si>
+  <si>
+    <t>(0.54)</t>
+  </si>
+  <si>
+    <t>(0.76)</t>
+  </si>
+  <si>
+    <t>(0.08)</t>
+  </si>
+  <si>
+    <t>(0.04)</t>
+  </si>
+  <si>
+    <t>(0.37)</t>
+  </si>
+  <si>
+    <t>(0.92)</t>
+  </si>
+  <si>
+    <t>(0.6)</t>
   </si>
   <si>
     <t>(0.38)</t>
-  </si>
-  <si>
-    <t>(0.97)</t>
   </si>
 </sst>
 </file>
@@ -586,22 +589,22 @@
         <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="J4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="K4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -659,25 +662,25 @@
         <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="L6" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:12">

</xml_diff>